<commit_message>
Atualizado com base nas interfaces
</commit_message>
<xml_diff>
--- a/Descrição de cado de uso - Cadastro Cliente.xlsx
+++ b/Descrição de cado de uso - Cadastro Cliente.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinicius\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heckl\Desktop\dev-sis-02-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA456C2E-2E38-467E-9876-BDF0335C8558}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949B9D7B-A77D-4BD4-AF28-37FE2EEDCC43}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{10E0717D-1ED4-48D6-BC75-4A327E9417D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{10E0717D-1ED4-48D6-BC75-4A327E9417D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> O Cliente começa a preencher o formulário de cadastro.                            
+      <t xml:space="preserve"> O Cliente acessa a página de cadastro.
 </t>
     </r>
     <r>
@@ -148,7 +148,51 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>1.1:</t>
+      <t>2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Seleciona o tipo de cadastro expecífico para cliente.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Começa a preencher o formulário de cadastro.                            
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3.1:</t>
     </r>
     <r>
       <rPr>
@@ -170,7 +214,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>1.2:</t>
+      <t>3.2:</t>
     </r>
     <r>
       <rPr>
@@ -192,7 +236,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>2:</t>
+      <t>4:</t>
     </r>
     <r>
       <rPr>
@@ -214,7 +258,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>2.1:</t>
+      <t>4.1:</t>
     </r>
     <r>
       <rPr>
@@ -236,7 +280,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>3:</t>
+      <t>5:</t>
     </r>
     <r>
       <rPr>
@@ -410,6 +454,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -422,24 +493,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -493,15 +546,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -820,7 +864,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="E15" sqref="E15:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,275 +873,278 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="7"/>
       <c r="G1" s="3"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="6"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10"/>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="8"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="17"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="15" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="17"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="20"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="20"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="23"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="15" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="17"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="20"/>
     </row>
     <row r="6" spans="1:11" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="21" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="23"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
     </row>
     <row r="8" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="26"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="15" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="20"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="20"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="23"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="15" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="20"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="20"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="21" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="23"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="26"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="29"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="27" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="29"/>
-    </row>
-    <row r="16" spans="1:11" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="32"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="32"/>
+    </row>
+    <row r="16" spans="1:11" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="35"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="27" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="29"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="32"/>
     </row>
     <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="32"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A7:C8"/>
+    <mergeCell ref="A9:C10"/>
+    <mergeCell ref="A11:C12"/>
     <mergeCell ref="A13:C14"/>
     <mergeCell ref="D3:D18"/>
     <mergeCell ref="A3:C4"/>
@@ -1114,9 +1161,6 @@
     <mergeCell ref="E13:K14"/>
     <mergeCell ref="E15:K16"/>
     <mergeCell ref="E17:K18"/>
-    <mergeCell ref="A7:C8"/>
-    <mergeCell ref="A9:C10"/>
-    <mergeCell ref="A11:C12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>